<commit_message>
feat: Change Scrap Sprrite
</commit_message>
<xml_diff>
--- a/DataBase/Data/Gathering.xlsx
+++ b/DataBase/Data/Gathering.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bangg\Desktop\Rookis\ExcelToJsonConverter\bin\Debug\net6.0\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Seoultech\Github\Unity\Project_G\DataBase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17316625-6411-4C4C-A4E6-A4DB94A41A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368F0A36-AA3B-4EAC-B939-FD8A9106841B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,15 +57,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rock</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bush</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scrap</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -393,13 +393,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -430,13 +432,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>30</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>5001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -458,7 +460,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>20</v>

</xml_diff>

<commit_message>
feat: add Monster DropItem
</commit_message>
<xml_diff>
--- a/DataBase/Data/Gathering.xlsx
+++ b/DataBase/Data/Gathering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Seoultech\Github\Unity\Project_G\DataBase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368F0A36-AA3B-4EAC-B939-FD8A9106841B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09C3948-D470-40FB-8E14-74C3952CED92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>5001</v>
+        <v>5101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
feat: Add Tileset and Items
</commit_message>
<xml_diff>
--- a/DataBase/Data/Gathering.xlsx
+++ b/DataBase/Data/Gathering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Seoultech\Github\Unity\Project_G\DataBase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09C3948-D470-40FB-8E14-74C3952CED92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10548B7-6AC4-46A9-9E5D-1077FD9FD8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,9 +397,9 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -413,7 +413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -427,7 +427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -438,10 +438,10 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>5101</v>
+        <v>4101</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -455,7 +455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>

</xml_diff>